<commit_message>
ultimas ediciones a etapa 3
</commit_message>
<xml_diff>
--- a/etapa3_tablas.xlsx
+++ b/etapa3_tablas.xlsx
@@ -462,10 +462,10 @@
         <v>0.09909999999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08150863215338089</v>
+        <v>0.08150863212614792</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7436556217682811</v>
+        <v>0.7436556217677459</v>
       </c>
     </row>
     <row r="3">
@@ -476,10 +476,10 @@
         <v>0.1669</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1568397720817122</v>
+        <v>0.1568405326489421</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5906164477442055</v>
+        <v>0.5906268483453735</v>
       </c>
     </row>
     <row r="4">
@@ -490,10 +490,10 @@
         <v>0.2374</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2346777859436837</v>
+        <v>0.2346779462782754</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4772223618573888</v>
+        <v>0.4772238367102605</v>
       </c>
     </row>
     <row r="5">
@@ -504,10 +504,10 @@
         <v>0.3013</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2975159217959192</v>
+        <v>0.3273595898062373</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2975159217959163</v>
+        <v>0.3701799637633356</v>
       </c>
     </row>
     <row r="6">
@@ -518,10 +518,10 @@
         <v>0.4026</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2975877305321012</v>
+        <v>0.3124981261414224</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2975877305320994</v>
+        <v>0.3855804851688722</v>
       </c>
     </row>
     <row r="7">
@@ -532,10 +532,10 @@
         <v>0.4984</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2940440606897718</v>
+        <v>0.2570425433549289</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2940440606989511</v>
+        <v>0.4490903601106034</v>
       </c>
     </row>
     <row r="8">
@@ -546,10 +546,10 @@
         <v>0.5964</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1655121294259377</v>
+        <v>0.1655040290119493</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5765058773679868</v>
+        <v>0.5764867229046448</v>
       </c>
     </row>
     <row r="9">
@@ -560,10 +560,10 @@
         <v>0.7245</v>
       </c>
       <c r="C9" t="n">
-        <v>0.08776700064651606</v>
+        <v>0.08776696834527142</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7273765656423214</v>
+        <v>0.727376560556585</v>
       </c>
     </row>
     <row r="10">
@@ -574,10 +574,10 @@
         <v>0.764</v>
       </c>
       <c r="C10" t="n">
-        <v>0.06636305378886369</v>
+        <v>0.06636296460780945</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7909866580668008</v>
+        <v>0.7909867264656207</v>
       </c>
     </row>
     <row r="11">
@@ -588,10 +588,10 @@
         <v>0.8919</v>
       </c>
       <c r="C11" t="n">
-        <v>0.07969206667662802</v>
+        <v>0.7245</v>
       </c>
       <c r="D11" t="n">
-        <v>0.87786843123634</v>
+        <v>0.09909999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>